<commit_message>
still working on data driven optimization
</commit_message>
<xml_diff>
--- a/Data Files/Footer/FooterDataColumns.xlsx
+++ b/Data Files/Footer/FooterDataColumns.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>header1</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>elementSet3</t>
+  </si>
+  <si>
+    <t>elementIndex</t>
   </si>
   <si>
     <t>About Us</t>
@@ -194,165 +197,192 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>